<commit_message>
Radiation integrator code completed
</commit_message>
<xml_diff>
--- a/reduced_data/radiation_data.xlsx
+++ b/reduced_data/radiation_data.xlsx
@@ -403,19 +403,19 @@
         <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>271.7204395340522</v>
+        <v>281.234939512093</v>
       </c>
       <c r="F3" t="n">
-        <v>267.3581800274297</v>
+        <v>267.3117925990559</v>
       </c>
       <c r="G3" t="n">
-        <v>-24.91475561932111</v>
+        <v>-1.430333635586761</v>
       </c>
       <c r="H3" t="n">
-        <v>9.205257252361982</v>
+        <v>0.4937534038465458</v>
       </c>
       <c r="I3" t="n">
-        <v>4.362259506622479</v>
+        <v>13.92314691303716</v>
       </c>
     </row>
   </sheetData>

</xml_diff>